<commit_message>
1. Update schematic to match with changes from Infiniti Solutions 2. Update BOM to remove socket and point to assemble P5
</commit_message>
<xml_diff>
--- a/docs/c19054_SALINAS_BOM.XLSX
+++ b/docs/c19054_SALINAS_BOM.XLSX
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anthony\GIT\personal\Salinas\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56074AD-9A0B-4B80-887C-8A6B82823882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49F92D1-A49A-4E20-8AFB-194E2953CC35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="290" yWindow="4630" windowWidth="23090" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14730" yWindow="1180" windowWidth="22930" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V1.1" sheetId="2" r:id="rId1"/>
-    <sheet name="V1.0" sheetId="1" r:id="rId2"/>
+    <sheet name="V1.11" sheetId="3" r:id="rId1"/>
+    <sheet name="V1.1" sheetId="2" r:id="rId2"/>
+    <sheet name="V1.0" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="226">
   <si>
     <t>Value</t>
   </si>
@@ -690,6 +691,15 @@
   </si>
   <si>
     <t>P1-P3,P5,P6</t>
+  </si>
+  <si>
+    <t>REV: 1.11 (09/14/20)</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>See change to line #33</t>
   </si>
 </sst>
 </file>
@@ -826,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -911,6 +921,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1249,14 +1271,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2762079A-DBD9-47F5-9BA1-1E2A76EB3735}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56150B89-571B-4166-83A4-80820A978496}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.1796875" defaultRowHeight="14.5"/>
@@ -1276,6 +1298,1149 @@
         <v>139</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="50.25" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11">
+        <v>61</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11">
+        <v>19</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="11">
+        <v>4</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>4</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29">
+      <c r="A10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29">
+      <c r="A12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="11">
+        <v>6</v>
+      </c>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="1:5" ht="29">
+      <c r="A19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="11">
+        <v>4</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="11">
+        <v>1</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="14">
+        <v>1</v>
+      </c>
+      <c r="E23" s="38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="14">
+        <v>2</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="14">
+        <v>1</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="14">
+        <v>1</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="14">
+        <v>1</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="14">
+        <v>4</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="14">
+        <v>1</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="14">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D33" s="14">
+        <v>5</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="14">
+        <v>13</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="14">
+        <v>2</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="14">
+        <v>4</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="14">
+        <v>18</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="D38" s="14">
+        <v>4</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" s="14">
+        <v>6</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="8" customFormat="1">
+      <c r="A40" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="14">
+        <v>9</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D41" s="14">
+        <v>5</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D42" s="14">
+        <v>8</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D43" s="14">
+        <v>13</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="11">
+        <v>1</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1</v>
+      </c>
+      <c r="E45" s="26"/>
+    </row>
+    <row r="46" spans="1:5" s="8" customFormat="1">
+      <c r="A46" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="14">
+        <v>13</v>
+      </c>
+      <c r="E46" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="11">
+        <v>3</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="11">
+        <v>2</v>
+      </c>
+      <c r="E48" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="11">
+        <v>4</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="D50" s="11">
+        <v>1</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="11">
+        <v>1</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="11">
+        <v>4</v>
+      </c>
+      <c r="E52" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="11">
+        <v>4</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D54" s="14">
+        <v>1</v>
+      </c>
+      <c r="E54" s="38"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D55" s="11">
+        <v>13</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="11">
+        <v>1</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="11">
+        <v>1</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" s="11">
+        <v>1</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="11">
+        <v>1</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="11">
+        <v>1</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" s="11">
+        <v>1</v>
+      </c>
+      <c r="E61" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D62" s="7">
+        <v>1</v>
+      </c>
+      <c r="E62" s="37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D64" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="D66" s="31">
+        <v>1</v>
+      </c>
+      <c r="E66" s="36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="49" fitToHeight="6" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2762079A-DBD9-47F5-9BA1-1E2A76EB3735}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26.1796875" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.7265625" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.5">
+      <c r="A1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>209</v>
       </c>
     </row>
@@ -2388,7 +3553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>